<commit_message>
Update Booking and SG data files with env data
</commit_message>
<xml_diff>
--- a/static/services/service_portfolio.xlsx
+++ b/static/services/service_portfolio.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hws/proj/bring/developer-site/static/services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24F033E-F502-F040-B6AD-E54C3E86573B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88103E58-DEBF-164F-A3DD-D3DDD45030D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33580" windowHeight="19480" xr2:uid="{D4AB77C3-6DE9-F04B-B545-B311CDF8D937}"/>
+    <workbookView xWindow="-44480" yWindow="-340" windowWidth="33580" windowHeight="19480" xr2:uid="{D4AB77C3-6DE9-F04B-B545-B311CDF8D937}"/>
   </bookViews>
   <sheets>
-    <sheet name="Booking &amp; SG API" sheetId="5" r:id="rId1"/>
+    <sheet name="Booking &amp; SG API" sheetId="6" r:id="rId1"/>
     <sheet name="Reports &amp; Invoice API" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="244">
   <si>
     <t>Service family</t>
   </si>
@@ -768,6 +768,9 @@
   </si>
   <si>
     <t>Express International 09:00</t>
+  </si>
+  <si>
+    <t>Environmental data</t>
   </si>
 </sst>
 </file>
@@ -1194,12 +1197,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457ED57F-AA50-6545-87C7-7B2DC3FDCD59}">
-  <dimension ref="A1:P63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830DC4F0-81D9-A84A-A4E6-14BBBA677375}">
+  <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1217,13 +1220,13 @@
     <col min="11" max="11" width="10.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="105.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="105.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16">
+    <row r="1" spans="1:17" ht="16">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1264,16 +1267,19 @@
         <v>16</v>
       </c>
       <c r="N1" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16">
+    <row r="2" spans="1:17" ht="16">
       <c r="A2" s="9" t="s">
         <v>29</v>
       </c>
@@ -1320,10 +1326,13 @@
         <v>45</v>
       </c>
       <c r="P2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16">
+    <row r="3" spans="1:17" ht="16">
       <c r="A3" s="9" t="s">
         <v>205</v>
       </c>
@@ -1364,16 +1373,19 @@
         <v>13</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="O3" s="9" t="s">
         <v>45</v>
       </c>
       <c r="P3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="16">
+    <row r="4" spans="1:17" ht="16">
       <c r="A4" s="9" t="s">
         <v>205</v>
       </c>
@@ -1414,16 +1426,19 @@
         <v>13</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="O4" s="9" t="s">
         <v>45</v>
       </c>
       <c r="P4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="16">
+    <row r="5" spans="1:17" ht="16">
       <c r="A5" s="9" t="s">
         <v>205</v>
       </c>
@@ -1470,10 +1485,13 @@
         <v>45</v>
       </c>
       <c r="P5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16">
+    <row r="6" spans="1:17" ht="16">
       <c r="A6" s="9" t="s">
         <v>205</v>
       </c>
@@ -1514,16 +1532,19 @@
         <v>13</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>45</v>
       </c>
       <c r="P6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q6" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="16">
+    <row r="7" spans="1:17" ht="16">
       <c r="A7" s="9" t="s">
         <v>205</v>
       </c>
@@ -1570,10 +1591,13 @@
         <v>45</v>
       </c>
       <c r="P7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q7" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="16">
+    <row r="8" spans="1:17" ht="16">
       <c r="A8" s="9" t="s">
         <v>205</v>
       </c>
@@ -1620,10 +1644,13 @@
         <v>45</v>
       </c>
       <c r="P8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q8" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="16">
+    <row r="9" spans="1:17" ht="16">
       <c r="A9" s="9" t="s">
         <v>205</v>
       </c>
@@ -1670,10 +1697,13 @@
         <v>45</v>
       </c>
       <c r="P9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q9" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="16">
+    <row r="10" spans="1:17" ht="16">
       <c r="A10" s="9" t="s">
         <v>205</v>
       </c>
@@ -1720,10 +1750,13 @@
         <v>45</v>
       </c>
       <c r="P10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="16">
+    <row r="11" spans="1:17" ht="16">
       <c r="A11" s="9" t="s">
         <v>205</v>
       </c>
@@ -1770,10 +1803,13 @@
         <v>45</v>
       </c>
       <c r="P11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q11" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="16">
+    <row r="12" spans="1:17" ht="16">
       <c r="A12" s="9" t="s">
         <v>43</v>
       </c>
@@ -1814,16 +1850,19 @@
         <v>13</v>
       </c>
       <c r="N12" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="O12" s="9" t="s">
+      <c r="P12" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="P12" s="9" t="s">
+      <c r="Q12" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="16">
+    <row r="13" spans="1:17" ht="16">
       <c r="A13" s="9" t="s">
         <v>205</v>
       </c>
@@ -1864,16 +1903,19 @@
         <v>13</v>
       </c>
       <c r="N13" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="O13" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="P13" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="P13" s="9" t="s">
+      <c r="Q13" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="16">
+    <row r="14" spans="1:17" ht="16">
       <c r="A14" s="9" t="s">
         <v>205</v>
       </c>
@@ -1914,16 +1956,19 @@
         <v>13</v>
       </c>
       <c r="N14" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="O14" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="O14" s="9" t="s">
+      <c r="P14" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="P14" s="9" t="s">
+      <c r="Q14" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="16">
+    <row r="15" spans="1:17" ht="16">
       <c r="A15" s="9" t="s">
         <v>205</v>
       </c>
@@ -1970,10 +2015,13 @@
         <v>45</v>
       </c>
       <c r="P15" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q15" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="16">
+    <row r="16" spans="1:17" ht="16">
       <c r="A16" s="9" t="s">
         <v>205</v>
       </c>
@@ -2014,16 +2062,19 @@
         <v>13</v>
       </c>
       <c r="N16" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="O16" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="O16" s="9" t="s">
+      <c r="P16" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="P16" s="9" t="s">
+      <c r="Q16" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="16">
+    <row r="17" spans="1:17" ht="16">
       <c r="A17" s="9" t="s">
         <v>205</v>
       </c>
@@ -2064,16 +2115,19 @@
         <v>13</v>
       </c>
       <c r="N17" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="O17" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="O17" s="9" t="s">
+      <c r="P17" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="P17" s="9" t="s">
+      <c r="Q17" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="16">
+    <row r="18" spans="1:17" ht="16">
       <c r="A18" s="9" t="s">
         <v>205</v>
       </c>
@@ -2120,10 +2174,13 @@
         <v>45</v>
       </c>
       <c r="P18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q18" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="16">
+    <row r="19" spans="1:17" ht="16">
       <c r="A19" s="9" t="s">
         <v>205</v>
       </c>
@@ -2164,16 +2221,19 @@
         <v>13</v>
       </c>
       <c r="N19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O19" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="O19" s="9" t="s">
+      <c r="P19" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="P19" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="16">
+      <c r="Q19" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="16">
       <c r="A20" s="9" t="s">
         <v>205</v>
       </c>
@@ -2214,16 +2274,19 @@
         <v>13</v>
       </c>
       <c r="N20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O20" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="O20" s="9" t="s">
+      <c r="P20" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="P20" s="9" t="s">
+      <c r="Q20" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="16">
+    <row r="21" spans="1:17" ht="16">
       <c r="A21" s="9" t="s">
         <v>205</v>
       </c>
@@ -2264,16 +2327,19 @@
         <v>13</v>
       </c>
       <c r="N21" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O21" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="O21" s="9" t="s">
+      <c r="P21" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="P21" s="9" t="s">
+      <c r="Q21" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="16">
+    <row r="22" spans="1:17" ht="16">
       <c r="A22" s="9" t="s">
         <v>205</v>
       </c>
@@ -2314,16 +2380,19 @@
         <v>13</v>
       </c>
       <c r="N22" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O22" s="9" t="s">
         <v>193</v>
-      </c>
-      <c r="O22" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="P22" s="9" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" ht="16">
+      <c r="Q22" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="16">
       <c r="A23" s="9" t="s">
         <v>205</v>
       </c>
@@ -2364,7 +2433,7 @@
         <v>13</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="O23" s="9" t="s">
         <v>74</v>
@@ -2372,8 +2441,11 @@
       <c r="P23" s="9" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" ht="16">
+      <c r="Q23" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="16">
       <c r="A24" s="9" t="s">
         <v>205</v>
       </c>
@@ -2414,7 +2486,7 @@
         <v>13</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="O24" s="9" t="s">
         <v>74</v>
@@ -2422,8 +2494,11 @@
       <c r="P24" s="9" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" ht="16">
+      <c r="Q24" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="16">
       <c r="A25" s="9" t="s">
         <v>205</v>
       </c>
@@ -2464,7 +2539,7 @@
         <v>13</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="O25" s="9" t="s">
         <v>74</v>
@@ -2472,8 +2547,11 @@
       <c r="P25" s="9" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" ht="16">
+      <c r="Q25" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="16">
       <c r="A26" s="9" t="s">
         <v>205</v>
       </c>
@@ -2514,7 +2592,7 @@
         <v>13</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="O26" s="9" t="s">
         <v>74</v>
@@ -2522,8 +2600,11 @@
       <c r="P26" s="9" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" ht="16">
+      <c r="Q26" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="16">
       <c r="A27" s="9" t="s">
         <v>25</v>
       </c>
@@ -2570,10 +2651,13 @@
         <v>45</v>
       </c>
       <c r="P27" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q27" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="16">
+    <row r="28" spans="1:17" ht="16">
       <c r="A28" s="9" t="s">
         <v>205</v>
       </c>
@@ -2620,10 +2704,13 @@
         <v>45</v>
       </c>
       <c r="P28" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q28" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="16">
+    <row r="29" spans="1:17" ht="16">
       <c r="A29" s="9" t="s">
         <v>205</v>
       </c>
@@ -2670,10 +2757,13 @@
         <v>45</v>
       </c>
       <c r="P29" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q29" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="16">
+    <row r="30" spans="1:17" ht="16">
       <c r="A30" s="9" t="s">
         <v>205</v>
       </c>
@@ -2720,10 +2810,13 @@
         <v>45</v>
       </c>
       <c r="P30" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q30" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="16">
+    <row r="31" spans="1:17" ht="16">
       <c r="A31" s="9" t="s">
         <v>2</v>
       </c>
@@ -2770,10 +2863,13 @@
         <v>45</v>
       </c>
       <c r="P31" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q31" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="16">
+    <row r="32" spans="1:17" ht="16">
       <c r="A32" s="9" t="s">
         <v>205</v>
       </c>
@@ -2820,10 +2916,13 @@
         <v>45</v>
       </c>
       <c r="P32" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q32" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="16">
+    <row r="33" spans="1:17" ht="16">
       <c r="A33" s="9" t="s">
         <v>205</v>
       </c>
@@ -2870,10 +2969,13 @@
         <v>45</v>
       </c>
       <c r="P33" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q33" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="16">
+    <row r="34" spans="1:17" ht="16">
       <c r="A34" s="9" t="s">
         <v>205</v>
       </c>
@@ -2920,10 +3022,13 @@
         <v>45</v>
       </c>
       <c r="P34" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q34" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="16">
+    <row r="35" spans="1:17" ht="16">
       <c r="A35" s="9" t="s">
         <v>205</v>
       </c>
@@ -2964,16 +3069,19 @@
         <v>13</v>
       </c>
       <c r="N35" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O35" s="9" t="s">
         <v>193</v>
-      </c>
-      <c r="O35" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="P35" s="9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" ht="16">
+      <c r="Q35" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="16">
       <c r="A36" s="9" t="s">
         <v>205</v>
       </c>
@@ -3020,10 +3128,13 @@
         <v>45</v>
       </c>
       <c r="P36" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q36" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="16">
+    <row r="37" spans="1:17" ht="16">
       <c r="A37" s="9" t="s">
         <v>205</v>
       </c>
@@ -3070,10 +3181,13 @@
         <v>45</v>
       </c>
       <c r="P37" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q37" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="16">
+    <row r="38" spans="1:17" ht="16">
       <c r="A38" s="9" t="s">
         <v>205</v>
       </c>
@@ -3120,10 +3234,13 @@
         <v>45</v>
       </c>
       <c r="P38" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q38" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="16">
+    <row r="39" spans="1:17" ht="16">
       <c r="A39" s="9" t="s">
         <v>93</v>
       </c>
@@ -3170,10 +3287,13 @@
         <v>45</v>
       </c>
       <c r="P39" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q39" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="16">
+    <row r="40" spans="1:17" ht="16">
       <c r="A40" s="9" t="s">
         <v>205</v>
       </c>
@@ -3220,10 +3340,13 @@
         <v>45</v>
       </c>
       <c r="P40" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q40" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="16">
+    <row r="41" spans="1:17" ht="16">
       <c r="A41" s="9" t="s">
         <v>205</v>
       </c>
@@ -3270,10 +3393,13 @@
         <v>45</v>
       </c>
       <c r="P41" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q41" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="16">
+    <row r="42" spans="1:17" ht="16">
       <c r="A42" s="9" t="s">
         <v>205</v>
       </c>
@@ -3320,10 +3446,13 @@
         <v>45</v>
       </c>
       <c r="P42" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q42" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="16">
+    <row r="43" spans="1:17" ht="16">
       <c r="A43" s="9" t="s">
         <v>205</v>
       </c>
@@ -3370,10 +3499,13 @@
         <v>45</v>
       </c>
       <c r="P43" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q43" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="16">
+    <row r="44" spans="1:17" ht="16">
       <c r="A44" s="9" t="s">
         <v>205</v>
       </c>
@@ -3420,10 +3552,13 @@
         <v>45</v>
       </c>
       <c r="P44" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q44" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="16">
+    <row r="45" spans="1:17" ht="16">
       <c r="A45" s="9" t="s">
         <v>205</v>
       </c>
@@ -3470,10 +3605,13 @@
         <v>45</v>
       </c>
       <c r="P45" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q45" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="16">
+    <row r="46" spans="1:17" ht="16">
       <c r="A46" s="9" t="s">
         <v>205</v>
       </c>
@@ -3520,10 +3658,13 @@
         <v>45</v>
       </c>
       <c r="P46" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q46" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="16">
+    <row r="47" spans="1:17" ht="16">
       <c r="A47" s="9" t="s">
         <v>205</v>
       </c>
@@ -3570,10 +3711,13 @@
         <v>45</v>
       </c>
       <c r="P47" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q47" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="16">
+    <row r="48" spans="1:17" ht="16">
       <c r="A48" s="9" t="s">
         <v>205</v>
       </c>
@@ -3620,10 +3764,13 @@
         <v>45</v>
       </c>
       <c r="P48" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q48" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="16">
+    <row r="49" spans="1:17" ht="16">
       <c r="A49" s="9" t="s">
         <v>205</v>
       </c>
@@ -3670,10 +3817,13 @@
         <v>45</v>
       </c>
       <c r="P49" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q49" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="16">
+    <row r="50" spans="1:17" ht="16">
       <c r="A50" s="9" t="s">
         <v>205</v>
       </c>
@@ -3714,16 +3864,19 @@
         <v>13</v>
       </c>
       <c r="N50" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O50" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="O50" s="9" t="s">
+      <c r="P50" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="P50" s="9" t="s">
+      <c r="Q50" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="16">
+    <row r="51" spans="1:17" ht="16">
       <c r="A51" s="9" t="s">
         <v>205</v>
       </c>
@@ -3764,16 +3917,19 @@
         <v>13</v>
       </c>
       <c r="N51" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O51" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="O51" s="9" t="s">
+      <c r="P51" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="P51" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" ht="16">
+      <c r="Q51" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="16">
       <c r="A52" s="9" t="s">
         <v>205</v>
       </c>
@@ -3814,16 +3970,19 @@
         <v>13</v>
       </c>
       <c r="N52" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O52" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="O52" s="9" t="s">
+      <c r="P52" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="P52" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" ht="16">
+      <c r="Q52" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="16">
       <c r="A53" s="9" t="s">
         <v>205</v>
       </c>
@@ -3864,16 +4023,19 @@
         <v>13</v>
       </c>
       <c r="N53" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O53" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="O53" s="9" t="s">
+      <c r="P53" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="P53" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" ht="16">
+      <c r="Q53" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" ht="16">
       <c r="A54" s="9" t="s">
         <v>205</v>
       </c>
@@ -3914,16 +4076,19 @@
         <v>13</v>
       </c>
       <c r="N54" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O54" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="O54" s="9" t="s">
+      <c r="P54" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="P54" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" ht="16">
+      <c r="Q54" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" ht="16">
       <c r="A55" s="9" t="s">
         <v>3</v>
       </c>
@@ -3964,16 +4129,19 @@
         <v>45</v>
       </c>
       <c r="N55" s="9" t="s">
-        <v>194</v>
+        <v>45</v>
       </c>
       <c r="O55" s="9" t="s">
         <v>194</v>
       </c>
       <c r="P55" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" ht="16">
+        <v>194</v>
+      </c>
+      <c r="Q55" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" ht="16">
       <c r="A56" s="9" t="s">
         <v>237</v>
       </c>
@@ -4020,10 +4188,13 @@
         <v>45</v>
       </c>
       <c r="P56" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q56" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="16">
+    <row r="57" spans="1:17" ht="16">
       <c r="A57" s="9" t="s">
         <v>4</v>
       </c>
@@ -4070,10 +4241,13 @@
         <v>45</v>
       </c>
       <c r="P57" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q57" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="16">
+    <row r="58" spans="1:17" ht="16">
       <c r="A58" s="9" t="s">
         <v>205</v>
       </c>
@@ -4122,8 +4296,11 @@
       <c r="P58" s="9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" ht="16">
+      <c r="Q58" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="16">
       <c r="A59" s="9" t="s">
         <v>205</v>
       </c>
@@ -4172,23 +4349,26 @@
       <c r="P59" s="9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="60" spans="1:16">
+      <c r="Q59" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17">
       <c r="A60" s="8" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:17">
       <c r="A61" s="8" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="16">
+    <row r="62" spans="1:17" ht="16">
       <c r="A62" s="7" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="16">
+    <row r="63" spans="1:17" ht="16">
       <c r="A63" s="9" t="s">
         <v>155</v>
       </c>
@@ -4984,6 +5164,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A896A3DCC9652247A91CA29CEC2FED62" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="379c2a5c320627d9e26f0b52d18a69ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6d43a431-f7e3-453d-9c03-0a38d302be99" xmlns:ns3="848c7fa4-5715-4bc0-ac9f-fcce6eb629b0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6623597d52b6039822fd09cbe50931f" ns2:_="" ns3:_="">
     <xsd:import namespace="6d43a431-f7e3-453d-9c03-0a38d302be99"/>
@@ -5188,36 +5383,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42AA1C04-6631-4B81-A064-6E275EC50E7B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{838419DF-55D5-4CA2-9755-AE1CB74AAB6F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6d43a431-f7e3-453d-9c03-0a38d302be99"/>
-    <ds:schemaRef ds:uri="848c7fa4-5715-4bc0-ac9f-fcce6eb629b0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5240,9 +5409,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{838419DF-55D5-4CA2-9755-AE1CB74AAB6F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42AA1C04-6631-4B81-A064-6E275EC50E7B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6d43a431-f7e3-453d-9c03-0a38d302be99"/>
+    <ds:schemaRef ds:uri="848c7fa4-5715-4bc0-ac9f-fcce6eb629b0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Set environmental support on 3570
</commit_message>
<xml_diff>
--- a/static/services/service_portfolio.xlsx
+++ b/static/services/service_portfolio.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hws/proj/bring/developer-site/static/services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88103E58-DEBF-164F-A3DD-D3DDD45030D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602EB450-E21F-8042-AEA3-932B82871C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44480" yWindow="-340" windowWidth="33580" windowHeight="19480" xr2:uid="{D4AB77C3-6DE9-F04B-B545-B311CDF8D937}"/>
+    <workbookView xWindow="-240" yWindow="600" windowWidth="33580" windowHeight="19480" xr2:uid="{D4AB77C3-6DE9-F04B-B545-B311CDF8D937}"/>
   </bookViews>
   <sheets>
-    <sheet name="Booking &amp; SG API" sheetId="6" r:id="rId1"/>
+    <sheet name="Booking &amp; SG API" sheetId="7" r:id="rId1"/>
     <sheet name="Reports &amp; Invoice API" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -1197,12 +1197,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830DC4F0-81D9-A84A-A4E6-14BBBA677375}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E47E0D-81DA-E244-8EF9-FE3D9263350C}">
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1479,7 +1479,7 @@
         <v>13</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>45</v>
@@ -5164,18 +5164,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5384,14 +5384,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{838419DF-55D5-4CA2-9755-AE1CB74AAB6F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{472388E6-C08A-4511-A70E-5CCA0082CECD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -5404,6 +5396,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{838419DF-55D5-4CA2-9755-AE1CB74AAB6F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update service table data sources
</commit_message>
<xml_diff>
--- a/static/services/service_portfolio.xlsx
+++ b/static/services/service_portfolio.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hws/proj/bring/developer-site/static/services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602EB450-E21F-8042-AEA3-932B82871C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3C9432-74E2-4947-838A-B10D0C9A4E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-240" yWindow="600" windowWidth="33580" windowHeight="19480" xr2:uid="{D4AB77C3-6DE9-F04B-B545-B311CDF8D937}"/>
+    <workbookView xWindow="-45080" yWindow="-600" windowWidth="33580" windowHeight="19480" xr2:uid="{D4AB77C3-6DE9-F04B-B545-B311CDF8D937}"/>
   </bookViews>
   <sheets>
-    <sheet name="Booking &amp; SG API" sheetId="7" r:id="rId1"/>
+    <sheet name="Booking &amp; SG API" sheetId="8" r:id="rId1"/>
     <sheet name="Reports &amp; Invoice API" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="245">
   <si>
     <t>Service family</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Retur fra hentested</t>
   </si>
   <si>
-    <t>C2B</t>
-  </si>
-  <si>
     <t>Retur pakke fra bedrift</t>
   </si>
   <si>
@@ -771,6 +768,12 @@
   </si>
   <si>
     <t>Environmental data</t>
+  </si>
+  <si>
+    <t>B2C return</t>
+  </si>
+  <si>
+    <t>B2B return</t>
   </si>
 </sst>
 </file>
@@ -1197,12 +1200,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E47E0D-81DA-E244-8EF9-FE3D9263350C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C98EFD-4914-9F41-A2DD-E29DA07A7B04}">
   <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1212,7 +1215,7 @@
     <col min="3" max="3" width="32.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" style="8" bestFit="1" customWidth="1"/>
@@ -1240,19 +1243,19 @@
         <v>7</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>12</v>
@@ -1267,7 +1270,7 @@
         <v>16</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>22</v>
@@ -1290,22 +1293,22 @@
         <v>8</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>13</v>
@@ -1320,13 +1323,13 @@
         <v>13</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>26</v>
@@ -1334,31 +1337,31 @@
     </row>
     <row r="3" spans="1:17" ht="16">
       <c r="A3" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>13</v>
@@ -1376,10 +1379,10 @@
         <v>26</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="9" t="s">
         <v>26</v>
@@ -1387,31 +1390,31 @@
     </row>
     <row r="4" spans="1:17" ht="16">
       <c r="A4" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>13</v>
@@ -1429,10 +1432,10 @@
         <v>26</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q4" s="9" t="s">
         <v>26</v>
@@ -1440,31 +1443,31 @@
     </row>
     <row r="5" spans="1:17" ht="16">
       <c r="A5" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>13</v>
@@ -1482,10 +1485,10 @@
         <v>26</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q5" s="9" t="s">
         <v>26</v>
@@ -1493,31 +1496,31 @@
     </row>
     <row r="6" spans="1:17" ht="16">
       <c r="A6" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>13</v>
@@ -1535,10 +1538,10 @@
         <v>26</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q6" s="9" t="s">
         <v>26</v>
@@ -1546,31 +1549,31 @@
     </row>
     <row r="7" spans="1:17" ht="16">
       <c r="A7" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>13</v>
@@ -1585,13 +1588,13 @@
         <v>13</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q7" s="9" t="s">
         <v>26</v>
@@ -1599,22 +1602,22 @@
     </row>
     <row r="8" spans="1:17" ht="16">
       <c r="A8" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>39</v>
+        <v>243</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>13</v>
@@ -1623,7 +1626,7 @@
         <v>13</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>13</v>
@@ -1638,13 +1641,13 @@
         <v>13</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q8" s="9" t="s">
         <v>26</v>
@@ -1652,22 +1655,22 @@
     </row>
     <row r="9" spans="1:17" ht="16">
       <c r="A9" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>39</v>
+        <v>243</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>13</v>
@@ -1676,7 +1679,7 @@
         <v>13</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>13</v>
@@ -1691,13 +1694,13 @@
         <v>13</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q9" s="9" t="s">
         <v>26</v>
@@ -1705,22 +1708,22 @@
     </row>
     <row r="10" spans="1:17" ht="16">
       <c r="A10" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>13</v>
@@ -1729,7 +1732,7 @@
         <v>13</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>13</v>
@@ -1744,13 +1747,13 @@
         <v>13</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q10" s="9" t="s">
         <v>26</v>
@@ -1758,22 +1761,22 @@
     </row>
     <row r="11" spans="1:17" ht="16">
       <c r="A11" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>13</v>
@@ -1782,7 +1785,7 @@
         <v>13</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>13</v>
@@ -1797,13 +1800,13 @@
         <v>13</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P11" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q11" s="9" t="s">
         <v>26</v>
@@ -1811,31 +1814,31 @@
     </row>
     <row r="12" spans="1:17" ht="16">
       <c r="A12" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>13</v>
@@ -1850,39 +1853,39 @@
         <v>13</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O12" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q12" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="P12" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q12" s="9" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="16">
       <c r="A13" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>13</v>
@@ -1894,48 +1897,48 @@
         <v>13</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M13" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q13" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="O13" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="P13" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q13" s="9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="16">
       <c r="A14" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>51</v>
-      </c>
       <c r="E14" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>13</v>
@@ -1956,51 +1959,51 @@
         <v>13</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P14" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q14" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="Q14" s="9" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="16">
       <c r="A15" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>13</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L15" s="9" t="s">
         <v>13</v>
@@ -2009,45 +2012,45 @@
         <v>13</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="16">
       <c r="A16" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>53</v>
-      </c>
       <c r="E16" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>13</v>
@@ -2062,39 +2065,39 @@
         <v>13</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P16" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="16">
       <c r="A17" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>55</v>
-      </c>
       <c r="E17" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>13</v>
@@ -2106,54 +2109,54 @@
         <v>13</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M17" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="16">
       <c r="A18" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C18" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>57</v>
-      </c>
       <c r="E18" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>13</v>
@@ -2168,39 +2171,39 @@
         <v>13</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P18" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="16">
       <c r="A19" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C19" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>59</v>
-      </c>
       <c r="E19" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>13</v>
@@ -2212,54 +2215,54 @@
         <v>13</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M19" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P19" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="16">
       <c r="A20" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C20" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="E20" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>13</v>
@@ -2274,45 +2277,45 @@
         <v>13</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P20" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="16">
       <c r="A21" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>13</v>
@@ -2327,45 +2330,45 @@
         <v>13</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="16">
       <c r="A22" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J22" s="9" t="s">
         <v>13</v>
@@ -2380,36 +2383,36 @@
         <v>13</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P22" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q22" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="16">
       <c r="A23" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C23" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>66</v>
-      </c>
       <c r="E23" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>39</v>
+        <v>243</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>13</v>
@@ -2424,45 +2427,45 @@
         <v>13</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M23" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P23" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="16">
       <c r="A24" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C24" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="E24" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>39</v>
+        <v>243</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>13</v>
@@ -2477,45 +2480,45 @@
         <v>13</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L24" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M24" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O24" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P24" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="16">
       <c r="A25" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>39</v>
+        <v>244</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>13</v>
@@ -2530,45 +2533,45 @@
         <v>13</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L25" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M25" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O25" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P25" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="16">
       <c r="A26" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C26" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>70</v>
-      </c>
       <c r="E26" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>13</v>
@@ -2583,25 +2586,25 @@
         <v>13</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M26" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="16">
@@ -2612,25 +2615,25 @@
         <v>30</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H27" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J27" s="9" t="s">
         <v>13</v>
@@ -2645,13 +2648,13 @@
         <v>13</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P27" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q27" s="9" t="s">
         <v>26</v>
@@ -2659,31 +2662,31 @@
     </row>
     <row r="28" spans="1:17" ht="16">
       <c r="A28" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>13</v>
@@ -2698,13 +2701,13 @@
         <v>13</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O28" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P28" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q28" s="9" t="s">
         <v>26</v>
@@ -2712,31 +2715,31 @@
     </row>
     <row r="29" spans="1:17" ht="16">
       <c r="A29" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H29" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J29" s="9" t="s">
         <v>13</v>
@@ -2751,13 +2754,13 @@
         <v>13</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P29" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q29" s="9" t="s">
         <v>26</v>
@@ -2765,22 +2768,22 @@
     </row>
     <row r="30" spans="1:17" ht="16">
       <c r="A30" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>13</v>
@@ -2789,7 +2792,7 @@
         <v>13</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J30" s="9" t="s">
         <v>13</v>
@@ -2804,13 +2807,13 @@
         <v>13</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P30" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q30" s="9" t="s">
         <v>26</v>
@@ -2824,281 +2827,281 @@
         <v>29</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D31" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="E31" s="9" t="s">
         <v>220</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>221</v>
       </c>
       <c r="F31" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J31" s="9" t="s">
         <v>13</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M31" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O31" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P31" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q31" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="16">
       <c r="A32" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H32" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J32" s="9" t="s">
         <v>13</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M32" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P32" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q32" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="16">
       <c r="A33" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J33" s="9" t="s">
         <v>13</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M33" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P33" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q33" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="16">
       <c r="A34" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J34" s="9" t="s">
         <v>13</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M34" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O34" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P34" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q34" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="16">
       <c r="A35" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H35" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J35" s="9" t="s">
         <v>13</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L35" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M35" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N35" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O35" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P35" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q35" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="16">
       <c r="A36" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>39</v>
+        <v>243</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>13</v>
@@ -3107,51 +3110,51 @@
         <v>13</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J36" s="9" t="s">
         <v>13</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L36" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M36" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N36" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O36" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P36" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q36" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="16">
       <c r="A37" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>39</v>
+        <v>243</v>
       </c>
       <c r="G37" s="9" t="s">
         <v>13</v>
@@ -3160,51 +3163,51 @@
         <v>13</v>
       </c>
       <c r="I37" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J37" s="9" t="s">
         <v>13</v>
       </c>
       <c r="K37" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L37" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M37" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O37" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P37" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q37" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="16">
       <c r="A38" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>39</v>
+        <v>243</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>13</v>
@@ -3213,60 +3216,60 @@
         <v>13</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J38" s="9" t="s">
         <v>13</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L38" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M38" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O38" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P38" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q38" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="16">
       <c r="A39" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B39" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>94</v>
-      </c>
       <c r="F39" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H39" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J39" s="9" t="s">
         <v>13</v>
@@ -3281,45 +3284,45 @@
         <v>13</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O39" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P39" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q39" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="16">
       <c r="A40" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H40" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J40" s="9" t="s">
         <v>13</v>
@@ -3334,45 +3337,45 @@
         <v>13</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O40" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P40" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q40" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="16">
       <c r="A41" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H41" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J41" s="9" t="s">
         <v>13</v>
@@ -3387,45 +3390,45 @@
         <v>13</v>
       </c>
       <c r="N41" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O41" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P41" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q41" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="16">
       <c r="A42" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J42" s="9" t="s">
         <v>13</v>
@@ -3440,45 +3443,45 @@
         <v>13</v>
       </c>
       <c r="N42" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O42" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P42" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q42" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="16">
       <c r="A43" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H43" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J43" s="9" t="s">
         <v>13</v>
@@ -3493,45 +3496,45 @@
         <v>13</v>
       </c>
       <c r="N43" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O43" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P43" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q43" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="16">
       <c r="A44" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>13</v>
@@ -3546,45 +3549,45 @@
         <v>13</v>
       </c>
       <c r="N44" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O44" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P44" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q44" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="16">
       <c r="A45" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H45" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I45" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J45" s="9" t="s">
         <v>13</v>
@@ -3599,45 +3602,45 @@
         <v>13</v>
       </c>
       <c r="N45" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O45" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P45" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q45" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="16">
       <c r="A46" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I46" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J46" s="9" t="s">
         <v>13</v>
@@ -3652,45 +3655,45 @@
         <v>13</v>
       </c>
       <c r="N46" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O46" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P46" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q46" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="16">
       <c r="A47" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H47" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I47" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J47" s="9" t="s">
         <v>13</v>
@@ -3705,45 +3708,45 @@
         <v>13</v>
       </c>
       <c r="N47" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O47" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P47" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q47" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="16">
       <c r="A48" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H48" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I48" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J48" s="9" t="s">
         <v>13</v>
@@ -3758,45 +3761,45 @@
         <v>13</v>
       </c>
       <c r="N48" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O48" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P48" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q48" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="16">
       <c r="A49" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H49" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J49" s="9" t="s">
         <v>13</v>
@@ -3805,51 +3808,51 @@
         <v>13</v>
       </c>
       <c r="L49" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M49" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N49" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O49" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P49" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q49" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="16">
       <c r="A50" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H50" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J50" s="9" t="s">
         <v>13</v>
@@ -3858,51 +3861,51 @@
         <v>13</v>
       </c>
       <c r="L50" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M50" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N50" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O50" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P50" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q50" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="16">
       <c r="A51" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H51" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J51" s="9" t="s">
         <v>13</v>
@@ -3911,51 +3914,51 @@
         <v>13</v>
       </c>
       <c r="L51" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M51" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N51" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O51" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P51" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q51" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="16">
       <c r="A52" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H52" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J52" s="9" t="s">
         <v>13</v>
@@ -3964,51 +3967,51 @@
         <v>13</v>
       </c>
       <c r="L52" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M52" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N52" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O52" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P52" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q52" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:17" ht="16">
       <c r="A53" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H53" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J53" s="9" t="s">
         <v>13</v>
@@ -4017,51 +4020,51 @@
         <v>13</v>
       </c>
       <c r="L53" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M53" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N53" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O53" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P53" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q53" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:17" ht="16">
       <c r="A54" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H54" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I54" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J54" s="9" t="s">
         <v>13</v>
@@ -4070,22 +4073,22 @@
         <v>13</v>
       </c>
       <c r="L54" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M54" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N54" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O54" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P54" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q54" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:17" ht="16">
@@ -4096,25 +4099,25 @@
         <v>3</v>
       </c>
       <c r="C55" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="E55" s="9" t="s">
         <v>144</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>145</v>
       </c>
       <c r="F55" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H55" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I55" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J55" s="9" t="s">
         <v>13</v>
@@ -4126,69 +4129,69 @@
         <v>13</v>
       </c>
       <c r="M55" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N55" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O55" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P55" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q55" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:17" ht="16">
       <c r="A56" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>28</v>
       </c>
       <c r="C56" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="E56" s="9" t="s">
         <v>146</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>147</v>
       </c>
       <c r="F56" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H56" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I56" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J56" s="9" t="s">
         <v>13</v>
       </c>
       <c r="K56" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L56" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M56" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N56" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O56" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P56" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q56" s="9" t="s">
         <v>26</v>
@@ -4199,28 +4202,28 @@
         <v>4</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I57" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J57" s="9" t="s">
         <v>13</v>
@@ -4229,19 +4232,19 @@
         <v>13</v>
       </c>
       <c r="L57" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M57" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N57" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O57" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P57" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q57" s="9" t="s">
         <v>26</v>
@@ -4249,31 +4252,31 @@
     </row>
     <row r="58" spans="1:17" ht="16">
       <c r="A58" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I58" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J58" s="9" t="s">
         <v>13</v>
@@ -4282,51 +4285,51 @@
         <v>13</v>
       </c>
       <c r="L58" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M58" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N58" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O58" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P58" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q58" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:17" ht="16">
       <c r="A59" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H59" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J59" s="9" t="s">
         <v>13</v>
@@ -4335,42 +4338,42 @@
         <v>13</v>
       </c>
       <c r="L59" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M59" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N59" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O59" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P59" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q59" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:17">
       <c r="A60" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="61" spans="1:17">
       <c r="A61" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="62" spans="1:17" ht="16">
       <c r="A62" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="63" spans="1:17" ht="16">
       <c r="A63" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -4432,10 +4435,10 @@
         <v>13</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -4444,7 +4447,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
       <c r="E3" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>21</v>
@@ -4456,10 +4459,10 @@
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
       <c r="E4" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -4468,10 +4471,10 @@
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
       <c r="E5" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -4480,10 +4483,10 @@
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
       <c r="E6" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4492,10 +4495,10 @@
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
       <c r="E7" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -4504,10 +4507,10 @@
       <c r="C8" s="2"/>
       <c r="D8" s="3"/>
       <c r="E8" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -4516,10 +4519,10 @@
       <c r="C9" s="2"/>
       <c r="D9" s="3"/>
       <c r="E9" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -4528,10 +4531,10 @@
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
       <c r="E10" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -4540,10 +4543,10 @@
       <c r="C11" s="2"/>
       <c r="D11" s="3"/>
       <c r="E11" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -4552,10 +4555,10 @@
       <c r="C12" s="2"/>
       <c r="D12" s="3"/>
       <c r="E12" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -4564,10 +4567,10 @@
       <c r="C13" s="2"/>
       <c r="D13" s="3"/>
       <c r="E13" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -4576,10 +4579,10 @@
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
       <c r="E14" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -4588,10 +4591,10 @@
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
       <c r="E15" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -4600,10 +4603,10 @@
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
       <c r="E16" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -4612,10 +4615,10 @@
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
       <c r="E17" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -4624,10 +4627,10 @@
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
       <c r="E18" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -4636,10 +4639,10 @@
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
       <c r="E19" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -4648,15 +4651,15 @@
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
       <c r="E20" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>30</v>
@@ -4668,10 +4671,10 @@
         <v>13</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -4680,7 +4683,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
       <c r="E22" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>21</v>
@@ -4692,10 +4695,10 @@
       <c r="C23" s="2"/>
       <c r="D23" s="3"/>
       <c r="E23" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -4704,10 +4707,10 @@
       <c r="C24" s="2"/>
       <c r="D24" s="3"/>
       <c r="E24" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -4716,10 +4719,10 @@
       <c r="C25" s="2"/>
       <c r="D25" s="3"/>
       <c r="E25" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -4728,10 +4731,10 @@
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
       <c r="E26" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -4740,10 +4743,10 @@
       <c r="C27" s="2"/>
       <c r="D27" s="3"/>
       <c r="E27" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -4752,10 +4755,10 @@
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
       <c r="E28" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -4764,10 +4767,10 @@
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
       <c r="E29" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -4776,10 +4779,10 @@
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
       <c r="E30" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -4788,10 +4791,10 @@
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
       <c r="E31" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -4800,10 +4803,10 @@
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
       <c r="E32" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -4812,10 +4815,10 @@
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
       <c r="E33" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -4824,10 +4827,10 @@
       <c r="C34" s="2"/>
       <c r="D34" s="3"/>
       <c r="E34" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -4836,10 +4839,10 @@
       <c r="C35" s="2"/>
       <c r="D35" s="3"/>
       <c r="E35" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -4848,10 +4851,10 @@
       <c r="C36" s="2"/>
       <c r="D36" s="3"/>
       <c r="E36" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -4860,10 +4863,10 @@
       <c r="C37" s="2"/>
       <c r="D37" s="3"/>
       <c r="E37" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -4880,10 +4883,10 @@
         <v>13</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -4892,7 +4895,7 @@
       <c r="C39" s="2"/>
       <c r="D39" s="3"/>
       <c r="E39" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>21</v>
@@ -4904,10 +4907,10 @@
       <c r="C40" s="2"/>
       <c r="D40" s="3"/>
       <c r="E40" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -4916,10 +4919,10 @@
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
       <c r="E41" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -4928,10 +4931,10 @@
       <c r="C42" s="2"/>
       <c r="D42" s="3"/>
       <c r="E42" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -4940,10 +4943,10 @@
       <c r="C43" s="2"/>
       <c r="D43" s="3"/>
       <c r="E43" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -4952,10 +4955,10 @@
       <c r="C44" s="2"/>
       <c r="D44" s="3"/>
       <c r="E44" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -4964,10 +4967,10 @@
       <c r="C45" s="2"/>
       <c r="D45" s="3"/>
       <c r="E45" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -4976,10 +4979,10 @@
       <c r="C46" s="2"/>
       <c r="D46" s="3"/>
       <c r="E46" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -4988,10 +4991,10 @@
       <c r="C47" s="2"/>
       <c r="D47" s="3"/>
       <c r="E47" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -5000,10 +5003,10 @@
       <c r="C48" s="2"/>
       <c r="D48" s="3"/>
       <c r="E48" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -5012,10 +5015,10 @@
       <c r="C49" s="2"/>
       <c r="D49" s="3"/>
       <c r="E49" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -5024,10 +5027,10 @@
       <c r="C50" s="2"/>
       <c r="D50" s="3"/>
       <c r="E50" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -5036,10 +5039,10 @@
       <c r="C51" s="2"/>
       <c r="D51" s="3"/>
       <c r="E51" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -5048,10 +5051,10 @@
       <c r="C52" s="2"/>
       <c r="D52" s="3"/>
       <c r="E52" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -5065,33 +5068,33 @@
         <v>13</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -5108,10 +5111,10 @@
         <v>13</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -5128,10 +5131,10 @@
         <v>13</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -5140,7 +5143,7 @@
       <c r="C57" s="2"/>
       <c r="D57" s="3"/>
       <c r="E57" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>21</v>
@@ -5152,10 +5155,10 @@
       <c r="C58" s="2"/>
       <c r="D58" s="3"/>
       <c r="E58" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -5164,21 +5167,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A896A3DCC9652247A91CA29CEC2FED62" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="379c2a5c320627d9e26f0b52d18a69ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6d43a431-f7e3-453d-9c03-0a38d302be99" xmlns:ns3="848c7fa4-5715-4bc0-ac9f-fcce6eb629b0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6623597d52b6039822fd09cbe50931f" ns2:_="" ns3:_="">
     <xsd:import namespace="6d43a431-f7e3-453d-9c03-0a38d302be99"/>
@@ -5383,32 +5371,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{472388E6-C08A-4511-A70E-5CCA0082CECD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="6d43a431-f7e3-453d-9c03-0a38d302be99"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="848c7fa4-5715-4bc0-ac9f-fcce6eb629b0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{838419DF-55D5-4CA2-9755-AE1CB74AAB6F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42AA1C04-6631-4B81-A064-6E275EC50E7B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5425,4 +5403,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{838419DF-55D5-4CA2-9755-AE1CB74AAB6F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{472388E6-C08A-4511-A70E-5CCA0082CECD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="6d43a431-f7e3-453d-9c03-0a38d302be99"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="848c7fa4-5715-4bc0-ac9f-fcce6eb629b0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Remove booking api from single indoor
</commit_message>
<xml_diff>
--- a/static/services/service_portfolio.xlsx
+++ b/static/services/service_portfolio.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hws/proj/bring/developer-site/static/services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3C9432-74E2-4947-838A-B10D0C9A4E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59B01F1-10DF-3E4D-9EA4-6653E2E95B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45080" yWindow="-600" windowWidth="33580" windowHeight="19480" xr2:uid="{D4AB77C3-6DE9-F04B-B545-B311CDF8D937}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" xr2:uid="{D4AB77C3-6DE9-F04B-B545-B311CDF8D937}"/>
   </bookViews>
   <sheets>
-    <sheet name="Booking &amp; SG API" sheetId="8" r:id="rId1"/>
+    <sheet name="Booking &amp; SG API" sheetId="9" r:id="rId1"/>
     <sheet name="Reports &amp; Invoice API" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -701,9 +701,6 @@
     <t>3150</t>
   </si>
   <si>
-    <t>SINGLE_INDOOR</t>
-  </si>
-  <si>
     <t>2870</t>
   </si>
   <si>
@@ -774,6 +771,9 @@
   </si>
   <si>
     <t>B2B return</t>
+  </si>
+  <si>
+    <t>SINGLE_INDOOR*</t>
   </si>
 </sst>
 </file>
@@ -1200,12 +1200,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C98EFD-4914-9F41-A2DD-E29DA07A7B04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E92B505-47D0-F242-9D84-2A06166A6CF2}">
   <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1270,7 +1270,7 @@
         <v>16</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>22</v>
@@ -1617,7 +1617,7 @@
         <v>210</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>13</v>
@@ -1670,7 +1670,7 @@
         <v>211</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>13</v>
@@ -1723,7 +1723,7 @@
         <v>212</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>13</v>
@@ -1776,7 +1776,7 @@
         <v>213</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>13</v>
@@ -2412,7 +2412,7 @@
         <v>133</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>13</v>
@@ -2465,7 +2465,7 @@
         <v>134</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>13</v>
@@ -2518,7 +2518,7 @@
         <v>135</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>13</v>
@@ -2571,7 +2571,7 @@
         <v>136</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>13</v>
@@ -2783,7 +2783,7 @@
         <v>218</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>13</v>
@@ -2833,7 +2833,7 @@
         <v>219</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="F31" s="9" t="s">
         <v>32</v>
@@ -2842,7 +2842,7 @@
         <v>44</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="I31" s="9" t="s">
         <v>84</v>
@@ -2883,7 +2883,7 @@
         <v>198</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>137</v>
@@ -2936,7 +2936,7 @@
         <v>199</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E33" s="9" t="s">
         <v>138</v>
@@ -2989,7 +2989,7 @@
         <v>200</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>139</v>
@@ -3042,10 +3042,10 @@
         <v>86</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>32</v>
@@ -3095,13 +3095,13 @@
         <v>87</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>140</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>13</v>
@@ -3148,13 +3148,13 @@
         <v>201</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>142</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G37" s="9" t="s">
         <v>13</v>
@@ -3201,13 +3201,13 @@
         <v>202</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>141</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>13</v>
@@ -3260,7 +3260,7 @@
         <v>93</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G39" s="9" t="s">
         <v>44</v>
@@ -3313,7 +3313,7 @@
         <v>94</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>44</v>
@@ -3366,7 +3366,7 @@
         <v>95</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G41" s="9" t="s">
         <v>44</v>
@@ -3419,7 +3419,7 @@
         <v>96</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>44</v>
@@ -3472,7 +3472,7 @@
         <v>102</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>44</v>
@@ -3525,7 +3525,7 @@
         <v>101</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>44</v>
@@ -3578,7 +3578,7 @@
         <v>97</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>44</v>
@@ -3631,7 +3631,7 @@
         <v>98</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>44</v>
@@ -3684,7 +3684,7 @@
         <v>99</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G47" s="9" t="s">
         <v>44</v>
@@ -3737,7 +3737,7 @@
         <v>100</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>44</v>
@@ -3787,10 +3787,10 @@
         <v>204</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G49" s="9" t="s">
         <v>44</v>
@@ -3837,13 +3837,13 @@
         <v>120</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>107</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>44</v>
@@ -3887,16 +3887,16 @@
         <v>204</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E51" s="9" t="s">
         <v>105</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G51" s="9" t="s">
         <v>44</v>
@@ -3943,13 +3943,13 @@
         <v>122</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>106</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G52" s="9" t="s">
         <v>44</v>
@@ -3996,13 +3996,13 @@
         <v>121</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>104</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G53" s="9" t="s">
         <v>44</v>
@@ -4049,13 +4049,13 @@
         <v>119</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E54" s="9" t="s">
         <v>103</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G54" s="9" t="s">
         <v>44</v>
@@ -4102,7 +4102,7 @@
         <v>143</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E55" s="9" t="s">
         <v>144</v>
@@ -4146,7 +4146,7 @@
     </row>
     <row r="56" spans="1:17" ht="16">
       <c r="A56" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>28</v>
@@ -4155,7 +4155,7 @@
         <v>145</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E56" s="9" t="s">
         <v>146</v>
@@ -4208,13 +4208,13 @@
         <v>4</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E57" s="9" t="s">
         <v>178</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G57" s="9" t="s">
         <v>44</v>
@@ -4261,13 +4261,13 @@
         <v>147</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>179</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G58" s="9" t="s">
         <v>44</v>
@@ -4314,13 +4314,13 @@
         <v>148</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>180</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G59" s="9" t="s">
         <v>44</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="62" spans="1:17" ht="16">
       <c r="A62" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="63" spans="1:17" ht="16">
@@ -5167,6 +5167,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A896A3DCC9652247A91CA29CEC2FED62" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="379c2a5c320627d9e26f0b52d18a69ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6d43a431-f7e3-453d-9c03-0a38d302be99" xmlns:ns3="848c7fa4-5715-4bc0-ac9f-fcce6eb629b0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6623597d52b6039822fd09cbe50931f" ns2:_="" ns3:_="">
     <xsd:import namespace="6d43a431-f7e3-453d-9c03-0a38d302be99"/>
@@ -5371,22 +5386,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{472388E6-C08A-4511-A70E-5CCA0082CECD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="6d43a431-f7e3-453d-9c03-0a38d302be99"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="848c7fa4-5715-4bc0-ac9f-fcce6eb629b0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{838419DF-55D5-4CA2-9755-AE1CB74AAB6F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42AA1C04-6631-4B81-A064-6E275EC50E7B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5403,29 +5428,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{838419DF-55D5-4CA2-9755-AE1CB74AAB6F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{472388E6-C08A-4511-A70E-5CCA0082CECD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="6d43a431-f7e3-453d-9c03-0a38d302be99"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="848c7fa4-5715-4bc0-ac9f-fcce6eb629b0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
improving the message about ALL countries except Russia and Belarus
</commit_message>
<xml_diff>
--- a/static/services/service_portfolio.xlsx
+++ b/static/services/service_portfolio.xlsx
@@ -176,7 +176,7 @@
     <t>NO, SE, DK, FI</t>
   </si>
   <si>
-    <t>NO, SE, DK, FI, AD, AE, AF, AG, AI, AL, AM, AN, AO, AQ, AR, AS, AT, AU, AW, AX, AZ, BA, BB, BD, BE, BF, BG, BH, BI, BJ, BL, BM, BN, BO, BQ, BR, BS, BT, BV, BW, BZ, CA, CC, CD, CF, CG, CH, CI, CK, CL, CM, CN, CO, CR, CU, CV, CW, CX, CY, CZ, DE, DJ, DM, DO, DZ, EC, EE, EG, EH, ER, ES, ET, FJ, FK, FM, FO, FR, GA, GB, GD, GE, GF, GG, GH, GI, GL, GM, GN, GP, GQ, GR, GS, GT, GU, GW, GY, HK, HM, HN, HR, HT, HU, ID, IE, IL, IM, IN, IO, IQ, IR, IS, IT, JE, JM, JO, JP, KE, KG, KH, KI, KM, KN, KP, KR, KW, KY, KZ, LA, LB, LC, LI, LK, LR, LS, LT, LU, LV, LY, MA, MC, MD, ME, MF, MG, MH, MK, ML, MM, MN, MO, MP, MQ, MR, MS, MT, MU, MV, MW, MX, MY, MZ, NA, NC, NE, NF, NG, NI, NL, NP, NR, NU, NZ, OM, PA, PE, PF, PG, PH, PK, PL, PM, PN, PR, PS, PT, PW, PY, QA, RE, RO, RS, RW, SA, SB, SC, SD, SG, SH, SI, SJ, SK, SL, SM, SN, SO, SR, SS, ST, SV, SX, SY, SZ, TC, TD, TF, TG, TH, TJ, TK, TL, TM, TN, TO, TR, TT, TV, TW, TZ, UA, UG, UM, US, UY, UZ, VA, VC, VE, VG, VI, VN, VU, WF, WS, XK, YE, YT, ZA, ZM, ZW</t>
+    <t>ALL COUNTRIES EXCEPT RUSSIA &amp; BELARUS</t>
   </si>
   <si>
     <t>PickUp Parcel Bulk</t>
@@ -816,7 +816,7 @@
     <col min="13" max="13" width="11.2890625" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="21.28125" customWidth="true" bestFit="true"/>
     <col min="15" max="15" width="18.5546875" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="107.359375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Document 9350 in API service portfolio
</commit_message>
<xml_diff>
--- a/static/services/service_portfolio.xlsx
+++ b/static/services/service_portfolio.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$66</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="215">
   <si>
     <t>Service family</t>
   </si>
@@ -137,6 +137,18 @@
     <t>B2C return</t>
   </si>
   <si>
+    <t>Retur til bedrift</t>
+  </si>
+  <si>
+    <t>9350</t>
+  </si>
+  <si>
+    <t>C2B return</t>
+  </si>
+  <si>
+    <t>Customer setup</t>
+  </si>
+  <si>
     <t>Retur pakke i postkassen</t>
   </si>
   <si>
@@ -333,9 +345,6 @@
   </si>
   <si>
     <t>5400</t>
-  </si>
-  <si>
-    <t>Customer setup</t>
   </si>
   <si>
     <t>Før 07:00 til bedrift</t>
@@ -795,7 +804,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q64"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -1263,7 +1272,7 @@
         <v>41</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>23</v>
@@ -1272,7 +1281,7 @@
         <v>23</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>23</v>
@@ -1307,16 +1316,16 @@
         <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>23</v>
@@ -1360,16 +1369,16 @@
         <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>23</v>
@@ -1407,25 +1416,25 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>23</v>
@@ -1446,33 +1455,33 @@
         <v>23</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>21</v>
@@ -1484,31 +1493,31 @@
         <v>23</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="Q13" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14">
@@ -1519,13 +1528,13 @@
         <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>21</v>
@@ -1537,31 +1546,31 @@
         <v>23</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="15">
@@ -1581,7 +1590,7 @@
         <v>67</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>22</v>
@@ -1590,7 +1599,7 @@
         <v>23</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>23</v>
@@ -1605,16 +1614,16 @@
         <v>23</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16">
@@ -1643,28 +1652,28 @@
         <v>23</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>72</v>
@@ -1696,31 +1705,31 @@
         <v>23</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -1731,13 +1740,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>34</v>
@@ -1749,16 +1758,16 @@
         <v>23</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>23</v>
@@ -1767,13 +1776,13 @@
         <v>22</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19">
@@ -1802,16 +1811,16 @@
         <v>23</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>23</v>
@@ -1820,13 +1829,13 @@
         <v>22</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>83</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20">
@@ -1840,10 +1849,10 @@
         <v>84</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>34</v>
@@ -1873,13 +1882,13 @@
         <v>22</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21">
@@ -1890,13 +1899,13 @@
         <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>34</v>
@@ -1926,13 +1935,13 @@
         <v>22</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22">
@@ -1943,34 +1952,34 @@
         <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>23</v>
@@ -1979,13 +1988,13 @@
         <v>22</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23">
@@ -2014,7 +2023,7 @@
         <v>23</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>23</v>
@@ -2032,13 +2041,13 @@
         <v>22</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24">
@@ -2049,26 +2058,26 @@
         <v>25</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="J24" s="1" t="s">
         <v>23</v>
       </c>
@@ -2085,13 +2094,13 @@
         <v>22</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25">
@@ -2102,16 +2111,16 @@
         <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>23</v>
@@ -2120,7 +2129,7 @@
         <v>23</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>23</v>
@@ -2138,21 +2147,21 @@
         <v>22</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>102</v>
@@ -2161,28 +2170,28 @@
         <v>103</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>23</v>
@@ -2191,30 +2200,30 @@
         <v>22</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>34</v>
@@ -2226,7 +2235,7 @@
         <v>23</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>106</v>
+        <v>22</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>23</v>
@@ -2261,10 +2270,10 @@
         <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>109</v>
@@ -2276,10 +2285,10 @@
         <v>22</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>23</v>
@@ -2320,7 +2329,7 @@
         <v>111</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>34</v>
@@ -2329,7 +2338,7 @@
         <v>22</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>22</v>
@@ -2367,19 +2376,19 @@
         <v>25</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>23</v>
@@ -2414,10 +2423,10 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>114</v>
+        <v>25</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>115</v>
@@ -2426,28 +2435,28 @@
         <v>116</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>106</v>
+        <v>22</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>23</v>
@@ -2456,21 +2465,21 @@
         <v>22</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>118</v>
@@ -2488,10 +2497,10 @@
         <v>22</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>23</v>
@@ -2509,13 +2518,13 @@
         <v>22</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33">
@@ -2544,7 +2553,7 @@
         <v>23</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>23</v>
@@ -2562,13 +2571,13 @@
         <v>22</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34">
@@ -2597,7 +2606,7 @@
         <v>23</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>23</v>
@@ -2615,13 +2624,13 @@
         <v>22</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35">
@@ -2638,7 +2647,7 @@
         <v>128</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>21</v>
@@ -2650,7 +2659,7 @@
         <v>23</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>23</v>
@@ -2668,13 +2677,13 @@
         <v>22</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36">
@@ -2685,25 +2694,25 @@
         <v>25</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>131</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>23</v>
@@ -2721,13 +2730,13 @@
         <v>22</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37">
@@ -2756,7 +2765,7 @@
         <v>23</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>23</v>
@@ -2774,13 +2783,13 @@
         <v>22</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38">
@@ -2809,7 +2818,7 @@
         <v>23</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>23</v>
@@ -2827,51 +2836,51 @@
         <v>22</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="F39" s="1" t="s">
-        <v>142</v>
+        <v>39</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M39" s="1" t="s">
         <v>23</v>
@@ -2880,34 +2889,34 @@
         <v>22</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>25</v>
+        <v>141</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>25</v>
+        <v>141</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="G40" s="1" t="s">
         <v>22</v>
       </c>
@@ -2939,7 +2948,7 @@
         <v>22</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41">
@@ -2959,7 +2968,7 @@
         <v>148</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>22</v>
@@ -2992,7 +3001,7 @@
         <v>22</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42">
@@ -3012,7 +3021,7 @@
         <v>151</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>22</v>
@@ -3045,7 +3054,7 @@
         <v>22</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43">
@@ -3065,7 +3074,7 @@
         <v>154</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>22</v>
@@ -3098,7 +3107,7 @@
         <v>22</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44">
@@ -3118,7 +3127,7 @@
         <v>157</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>22</v>
@@ -3151,7 +3160,7 @@
         <v>22</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45">
@@ -3171,7 +3180,7 @@
         <v>160</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>22</v>
@@ -3204,7 +3213,7 @@
         <v>22</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46">
@@ -3224,7 +3233,7 @@
         <v>163</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>22</v>
@@ -3257,7 +3266,7 @@
         <v>22</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47">
@@ -3277,7 +3286,7 @@
         <v>166</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>22</v>
@@ -3310,7 +3319,7 @@
         <v>22</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48">
@@ -3330,7 +3339,7 @@
         <v>169</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>22</v>
@@ -3363,7 +3372,7 @@
         <v>22</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49">
@@ -3377,13 +3386,13 @@
         <v>170</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>25</v>
+        <v>171</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>22</v>
@@ -3392,7 +3401,7 @@
         <v>23</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>106</v>
+        <v>22</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>23</v>
@@ -3401,10 +3410,10 @@
         <v>23</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N49" s="1" t="s">
         <v>22</v>
@@ -3416,7 +3425,7 @@
         <v>22</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50">
@@ -3427,16 +3436,16 @@
         <v>25</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>173</v>
+        <v>25</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>174</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>22</v>
@@ -3445,7 +3454,7 @@
         <v>23</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>23</v>
@@ -3457,19 +3466,19 @@
         <v>22</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N50" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51">
@@ -3489,7 +3498,7 @@
         <v>177</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>22</v>
@@ -3516,13 +3525,13 @@
         <v>22</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52">
@@ -3542,7 +3551,7 @@
         <v>180</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>22</v>
@@ -3569,10 +3578,10 @@
         <v>22</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="Q52" s="1" t="s">
         <v>22</v>
@@ -3595,7 +3604,7 @@
         <v>183</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>22</v>
@@ -3622,10 +3631,10 @@
         <v>22</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="Q53" s="1" t="s">
         <v>22</v>
@@ -3648,7 +3657,7 @@
         <v>186</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>22</v>
@@ -3675,10 +3684,10 @@
         <v>22</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="Q54" s="1" t="s">
         <v>22</v>
@@ -3686,22 +3695,22 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="F55" s="1" t="s">
-        <v>34</v>
+        <v>145</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>22</v>
@@ -3719,19 +3728,19 @@
         <v>23</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>191</v>
+        <v>55</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>191</v>
+        <v>62</v>
       </c>
       <c r="Q55" s="1" t="s">
         <v>22</v>
@@ -3739,19 +3748,19 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>34</v>
@@ -3769,51 +3778,51 @@
         <v>23</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>22</v>
+        <v>194</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>22</v>
+        <v>194</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C57" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>198</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>142</v>
+        <v>34</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>22</v>
@@ -3822,7 +3831,7 @@
         <v>23</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>22</v>
@@ -3845,7 +3854,7 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>25</v>
+        <v>199</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>25</v>
@@ -3860,7 +3869,7 @@
         <v>201</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>22</v>
@@ -3881,7 +3890,7 @@
         <v>22</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N58" s="1" t="s">
         <v>22</v>
@@ -3893,7 +3902,7 @@
         <v>22</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="59">
@@ -3913,7 +3922,7 @@
         <v>204</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>22</v>
@@ -3963,19 +3972,19 @@
         <v>206</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>106</v>
+        <v>22</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>23</v>
@@ -3993,37 +4002,90 @@
         <v>22</v>
       </c>
       <c r="O60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O61" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P60" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="Q60" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s">
-        <v>208</v>
+      <c r="P61" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q61" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="s" s="1">
-        <v>210</v>
+      <c r="A63" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="1">
-        <v>211</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="1">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P65"/>
+  <autoFilter ref="A1:P66"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>